<commit_message>
Data from Excel FIle
Read Data From Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fraz5\Documents\GitHub\A51-QA-Automation-Framework\A51-QA-Automation-Framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E3DBAB-E793-4180-BE24-0D9718904A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A37215-2E5B-4A49-B321-A7688AA97A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>test@test.com</t>
   </si>
   <si>
     <t>NoTest@noTest.com</t>
+  </si>
+  <si>
+    <t>sadasd@test.com</t>
+  </si>
+  <si>
+    <t>sdasdas@test.com</t>
+  </si>
+  <si>
+    <t>sadasdsf2@sad.com</t>
+  </si>
+  <si>
+    <t>sadqwetg@test.com</t>
   </si>
 </sst>
 </file>
@@ -359,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,10 +391,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{2808ED92-6D43-43AA-AEED-F28AD5A33CAF}"/>
     <hyperlink ref="B1" r:id="rId2" xr:uid="{0C06F3F3-FD97-4A99-8471-A7617ADD9AC8}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{1611DD6C-F887-49E6-BAD1-1A095BAE625A}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{957BC340-46AB-4547-AE8A-96ABDEA28868}"/>
+    <hyperlink ref="A3" r:id="rId5" xr:uid="{96A6E2EA-1EAC-46CF-887F-3F951AF0DE03}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{E1427D30-D39E-4382-8297-F3C170347A3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>